<commit_message>
Solver fixes: Change details: 1. Reworked region initialization. 2. Renamed Complete button to Check button.
BONUS:
3. Only one text hint per region (:
</commit_message>
<xml_diff>
--- a/KENKENNN/KENKENNN/Data/RegionData3.xlsx
+++ b/KENKENNN/KENKENNN/Data/RegionData3.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC38631-A557-4F2A-9B7B-4211F3C4E9E8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="10710" yWindow="1680" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>a</t>
   </si>
@@ -58,12 +59,18 @@
   </si>
   <si>
     <t>i</t>
+  </si>
+  <si>
+    <t>multi</t>
+  </si>
+  <si>
+    <t>sub</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -104,6 +111,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -152,7 +162,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -185,9 +195,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -220,6 +247,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -395,11 +439,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +488,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -471,7 +515,7 @@
         <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="K2" t="s">
         <v>12</v>
@@ -482,7 +526,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>9</v>
@@ -509,7 +553,7 @@
         <v>3</v>
       </c>
       <c r="J3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K3">
         <v>4</v>
@@ -524,7 +568,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -536,7 +580,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>